<commit_message>
figure update + si update
</commit_message>
<xml_diff>
--- a/data/iam_regions.xlsx
+++ b/data/iam_regions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marinaandrijevic/PhD/covid_recovery/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marinaandrijevic/PhD/covid_recovery/covid_recovery/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACC5C035-862D-5048-9FFA-D749B0D13909}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A691DFF8-0204-914C-A1D7-E6E0CF8F0DED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14780" yWindow="460" windowWidth="23620" windowHeight="18460" xr2:uid="{0EC8E63C-760B-AF4E-A7D5-B82DF59CBC06}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="188">
   <si>
     <t>Algeria</t>
   </si>
@@ -576,9 +576,6 @@
   </si>
   <si>
     <t>European Union</t>
-  </si>
-  <si>
-    <t>EU</t>
   </si>
   <si>
     <t>Uganda</t>
@@ -969,7 +966,7 @@
   <dimension ref="A1:B183"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A150" workbookViewId="0">
-      <selection activeCell="C181" sqref="C181"/>
+      <selection activeCell="B184" sqref="B184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -987,7 +984,7 @@
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -995,7 +992,7 @@
         <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -1003,7 +1000,7 @@
         <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -1011,7 +1008,7 @@
         <v>34</v>
       </c>
       <c r="B5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -1019,7 +1016,7 @@
         <v>39</v>
       </c>
       <c r="B6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -1027,7 +1024,7 @@
         <v>47</v>
       </c>
       <c r="B7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -1035,7 +1032,7 @@
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -1043,7 +1040,7 @@
         <v>58</v>
       </c>
       <c r="B9" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -1051,7 +1048,7 @@
         <v>25</v>
       </c>
       <c r="B10" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -1059,7 +1056,7 @@
         <v>35</v>
       </c>
       <c r="B11" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -1067,7 +1064,7 @@
         <v>40</v>
       </c>
       <c r="B12" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -1075,7 +1072,7 @@
         <v>48</v>
       </c>
       <c r="B13" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -1083,7 +1080,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -1091,7 +1088,7 @@
         <v>26</v>
       </c>
       <c r="B15" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -1099,7 +1096,7 @@
         <v>36</v>
       </c>
       <c r="B16" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -1107,7 +1104,7 @@
         <v>41</v>
       </c>
       <c r="B17" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -1115,7 +1112,7 @@
         <v>49</v>
       </c>
       <c r="B18" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -1123,7 +1120,7 @@
         <v>14</v>
       </c>
       <c r="B19" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -1131,7 +1128,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -1139,7 +1136,7 @@
         <v>27</v>
       </c>
       <c r="B21" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
@@ -1147,7 +1144,7 @@
         <v>37</v>
       </c>
       <c r="B22" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
@@ -1155,7 +1152,7 @@
         <v>42</v>
       </c>
       <c r="B23" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
@@ -1163,7 +1160,7 @@
         <v>50</v>
       </c>
       <c r="B24" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
@@ -1171,7 +1168,7 @@
         <v>20</v>
       </c>
       <c r="B25" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
@@ -1179,7 +1176,7 @@
         <v>28</v>
       </c>
       <c r="B26" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
@@ -1187,7 +1184,7 @@
         <v>38</v>
       </c>
       <c r="B27" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
@@ -1195,7 +1192,7 @@
         <v>43</v>
       </c>
       <c r="B28" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
@@ -1203,7 +1200,7 @@
         <v>21</v>
       </c>
       <c r="B29" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
@@ -1211,7 +1208,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
@@ -1219,7 +1216,7 @@
         <v>44</v>
       </c>
       <c r="B31" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
@@ -1227,7 +1224,7 @@
         <v>57</v>
       </c>
       <c r="B32" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
@@ -1235,7 +1232,7 @@
         <v>51</v>
       </c>
       <c r="B33" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
@@ -1243,7 +1240,7 @@
         <v>22</v>
       </c>
       <c r="B34" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
@@ -1251,7 +1248,7 @@
         <v>30</v>
       </c>
       <c r="B35" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
@@ -1259,7 +1256,7 @@
         <v>56</v>
       </c>
       <c r="B36" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
@@ -1267,7 +1264,7 @@
         <v>45</v>
       </c>
       <c r="B37" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
@@ -1275,7 +1272,7 @@
         <v>15</v>
       </c>
       <c r="B38" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
@@ -1283,7 +1280,7 @@
         <v>23</v>
       </c>
       <c r="B39" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
@@ -1291,7 +1288,7 @@
         <v>31</v>
       </c>
       <c r="B40" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
@@ -1299,7 +1296,7 @@
         <v>52</v>
       </c>
       <c r="B41" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
@@ -1307,7 +1304,7 @@
         <v>46</v>
       </c>
       <c r="B42" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
@@ -1315,7 +1312,7 @@
         <v>53</v>
       </c>
       <c r="B43" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
@@ -1323,7 +1320,7 @@
         <v>16</v>
       </c>
       <c r="B44" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
@@ -1331,7 +1328,7 @@
         <v>54</v>
       </c>
       <c r="B45" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
@@ -1339,7 +1336,7 @@
         <v>32</v>
       </c>
       <c r="B46" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
@@ -1347,7 +1344,7 @@
         <v>55</v>
       </c>
       <c r="B47" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
@@ -1355,7 +1352,7 @@
         <v>17</v>
       </c>
       <c r="B48" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
@@ -1363,7 +1360,7 @@
         <v>33</v>
       </c>
       <c r="B49" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
@@ -2128,7 +2125,7 @@
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B145" s="2" t="s">
         <v>145</v>
@@ -2136,7 +2133,7 @@
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B146" s="2" t="s">
         <v>145</v>
@@ -2144,7 +2141,7 @@
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B147" s="2" t="s">
         <v>145</v>
@@ -2160,7 +2157,7 @@
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B149" s="2" t="s">
         <v>145</v>
@@ -2168,7 +2165,7 @@
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B150" s="2" t="s">
         <v>145</v>
@@ -2176,7 +2173,7 @@
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B151" s="2" t="s">
         <v>145</v>
@@ -2435,7 +2432,7 @@
         <v>180</v>
       </c>
       <c r="B183" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>

</xml_diff>